<commit_message>
Add and edit some staffs
</commit_message>
<xml_diff>
--- a/devices.xlsx
+++ b/devices.xlsx
@@ -59,10 +59,10 @@
     <t>username + password</t>
   </si>
   <si>
+    <t>192.168.146.135</t>
+  </si>
+  <si>
     <t>telnet</t>
-  </si>
-  <si>
-    <t>192.168.146.100</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +417,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -432,7 +432,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>23</v>

</xml_diff>